<commit_message>
Added Web Table Handling + Non working code of writing data into excel
</commit_message>
<xml_diff>
--- a/BrowserTest/Data/Data.xlsx
+++ b/BrowserTest/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simra\Desktop\BrowserLibrary_RF\BrowserTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A6941D-02F0-471B-8492-74AE199F0108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F7BFD7-0FA3-49AA-9975-A1E837D26BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FB6C15AF-7C41-477E-8D9C-ACD2DC19F9AD}"/>
   </bookViews>
@@ -105,9 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,29 +427,29 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -458,7 +460,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -469,7 +471,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -480,7 +482,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -491,7 +493,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="A6" s="3">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -502,7 +504,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="A7" s="3">
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -513,7 +515,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="A8" s="3">
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -524,7 +526,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="A9" s="3">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -535,7 +537,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -546,7 +548,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="A11" s="3">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -557,7 +559,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+      <c r="A12" s="3">
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -568,7 +570,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="A13" s="3">
         <v>21</v>
       </c>
       <c r="B13" s="1" t="s">

</xml_diff>